<commit_message>
Add 10 KPIs on Overview Page & Add IMG Filter of Platform
</commit_message>
<xml_diff>
--- a/Documentation/data_dictionary.xlsx
+++ b/Documentation/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\Trump_Social_Media_Analysis\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AD38FF-C110-493F-8CDC-21D12EBAC84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25091028-FB4B-451B-B6C2-25534EE45381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A4286A7-6348-47EE-94B2-EC6D39D03C60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{3A4286A7-6348-47EE-94B2-EC6D39D03C60}"/>
   </bookViews>
   <sheets>
     <sheet name="Gathering Info of Columns" sheetId="2" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0A916-00A5-4A1A-9D59-3FCF1B9094C8}">
   <dimension ref="B3:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="A14" zoomScale="73" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1328,7 +1328,7 @@
         <v>18</v>
       </c>
       <c r="L6" s="7">
-        <f t="shared" ref="L6:L16" si="1">J6-K6</f>
+        <f t="shared" ref="L6:L11" si="1">J6-K6</f>
         <v>0</v>
       </c>
     </row>
@@ -1828,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1133A8B9-0B5E-4DDE-81E7-620C8AE7C0A7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Implemented Time Trend Analysis KPIs with engagement trends and MoM growth
</commit_message>
<xml_diff>
--- a/Documentation/data_dictionary.xlsx
+++ b/Documentation/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\Trump_Social_Media_Analysis\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25091028-FB4B-451B-B6C2-25534EE45381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659FB80C-1ABF-41AD-A8A5-D0DB3DEE2FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{3A4286A7-6348-47EE-94B2-EC6D39D03C60}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A4286A7-6348-47EE-94B2-EC6D39D03C60}"/>
   </bookViews>
   <sheets>
     <sheet name="Gathering Info of Columns" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>Befoe Transformation</t>
   </si>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E0A916-00A5-4A1A-9D59-3FCF1B9094C8}">
   <dimension ref="B3:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="73" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="73" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -943,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="62.4">
@@ -960,7 +960,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="46.8">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="31.2">
@@ -994,7 +994,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="62.4">
@@ -1011,7 +1011,7 @@
         <v>8</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="46.8">
@@ -1028,7 +1028,7 @@
         <v>9</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="46.8">
@@ -1045,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="46.8">
@@ -1062,7 +1062,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="46.8">
@@ -1079,7 +1079,7 @@
         <v>12</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="46.8">
@@ -1096,7 +1096,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="46.8">
@@ -1113,7 +1113,7 @@
         <v>14</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="46.8">
@@ -1129,8 +1129,8 @@
       <c r="G20" s="6">
         <v>15</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>22</v>
+      <c r="H20" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="31.2">
@@ -1147,7 +1147,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="46.8">
@@ -1164,7 +1164,7 @@
         <v>17</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="46.8">
@@ -1181,7 +1181,7 @@
         <v>18</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -1189,16 +1189,11 @@
         <v>19</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="2:8">
-      <c r="G25" s="6">
-        <v>20</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="2:8">
       <c r="H26" s="8"/>
@@ -1216,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806565-EFC0-4C60-A6D1-AD2DC5BA6196}">
-  <dimension ref="B4:L16"/>
+  <dimension ref="B4:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1317,7 +1312,7 @@
         <v>90343</v>
       </c>
       <c r="I6" s="7">
-        <f t="shared" ref="I6:I16" si="0">G6-H6</f>
+        <f t="shared" ref="I6:I17" si="0">G6-H6</f>
         <v>0</v>
       </c>
       <c r="J6" s="7">
@@ -1356,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="7">
-        <f t="shared" ref="J7:J16" si="3">K6</f>
+        <f t="shared" ref="J7:J17" si="3">K6</f>
         <v>18</v>
       </c>
       <c r="K7" s="7">
@@ -1454,7 +1449,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" ref="G10:G16" si="4">H9</f>
+        <f t="shared" ref="G10:G17" si="4">H9</f>
         <v>90343</v>
       </c>
       <c r="H10" s="7">
@@ -1692,6 +1687,44 @@
       <c r="L16" s="7">
         <v>1</v>
       </c>
+    </row>
+    <row r="17" spans="2:12" ht="15.6">
+      <c r="B17" s="7">
+        <v>12</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="7">
+        <v>12</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="4"/>
+        <v>90343</v>
+      </c>
+      <c r="H17" s="7">
+        <v>90343</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K17" s="7">
+        <v>19</v>
+      </c>
+      <c r="L17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="15.6">
+      <c r="B18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1700,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCDC835-0396-4215-9379-334408DE0CE0}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1819,6 +1852,17 @@
         <v>62</v>
       </c>
     </row>
+    <row r="13" spans="2:6" ht="15.6">
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1828,7 +1872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1133A8B9-0B5E-4DDE-81E7-620C8AE7C0A7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>

</xml_diff>